<commit_message>
Changed loudness + removed countdown to 1.5s pause
</commit_message>
<xml_diff>
--- a/Analysis/Sound_data.xlsx
+++ b/Analysis/Sound_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{377FCB5C-5A4C-4CC1-BF9A-8B06EAAA79CA}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{16A6E042-1AEA-4588-8CAD-87306327E470}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4362" uniqueCount="1482">
   <si>
     <t>Initial/NoRepeat/Droplet_B.wav</t>
   </si>
@@ -4452,12 +4452,6 @@
   </si>
   <si>
     <t>Growl_C.wav</t>
-  </si>
-  <si>
-    <t>Coin_B.wav</t>
-  </si>
-  <si>
-    <t>Coin_C.wav</t>
   </si>
   <si>
     <t>Goat_A.wav</t>
@@ -19707,8 +19701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F85263D-95D4-4235-A601-C901960AD746}">
   <dimension ref="A1:BO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D54" activeCellId="1" sqref="D52 D54"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19878,14 +19872,14 @@
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="F12" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.35">
@@ -19973,7 +19967,7 @@
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E22" t="s">
@@ -20003,7 +19997,7 @@
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E25" t="s">
@@ -20022,7 +20016,7 @@
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E27" t="s">
@@ -20072,7 +20066,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>75</v>
       </c>
@@ -20083,7 +20077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>76</v>
       </c>
@@ -20094,7 +20088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>77</v>
       </c>
@@ -20102,31 +20096,31 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>84</v>
       </c>
@@ -20137,21 +20131,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>1476</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1477</v>
-      </c>
+      <c r="D40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="13"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -20162,15 +20151,15 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -20178,26 +20167,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E44" t="s">
         <v>1472</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -20205,19 +20194,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E48" t="s">
@@ -20236,7 +20225,7 @@
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="12" t="s">
         <v>94</v>
       </c>
       <c r="E50" t="s">
@@ -20276,14 +20265,14 @@
       <c r="A52" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="11" t="s">
         <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="F52" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="G52">
         <v>20</v>
@@ -20299,8 +20288,8 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D53" s="1" t="s">
-        <v>81</v>
+      <c r="D53" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="G53">
         <v>50</v>
@@ -20313,14 +20302,14 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="F54" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated to Old-New Response version (still testing, not final)
</commit_message>
<xml_diff>
--- a/Analysis/Sound_data.xlsx
+++ b/Analysis/Sound_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{16A6E042-1AEA-4588-8CAD-87306327E470}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC5A8EB4-5B91-4E0E-9232-B4C1CD66717B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4362" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="1482">
   <si>
     <t>Initial/NoRepeat/Droplet_B.wav</t>
   </si>
@@ -5370,9 +5370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV93"/>
   <sheetViews>
-    <sheetView topLeftCell="BH1" workbookViewId="0">
+    <sheetView topLeftCell="BB1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BJ1" sqref="BJ1"/>
+      <selection pane="bottomLeft" activeCell="BH1" sqref="BH1:BH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19701,8 +19701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F85263D-95D4-4235-A601-C901960AD746}">
   <dimension ref="A1:BO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19720,7 +19720,9 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -19792,6 +19794,9 @@
       <c r="D2" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -19803,6 +19808,9 @@
       <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="11" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -19811,6 +19819,9 @@
       <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="G4" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -19819,6 +19830,9 @@
       <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
+      <c r="G5" s="11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -19827,6 +19841,9 @@
       <c r="D6" s="12" t="s">
         <v>61</v>
       </c>
+      <c r="G6" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -19835,6 +19852,9 @@
       <c r="D7" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="G7" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
@@ -19843,6 +19863,9 @@
       <c r="D8" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="G8" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -19851,6 +19874,9 @@
       <c r="D9" s="11" t="s">
         <v>76</v>
       </c>
+      <c r="G9" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -19859,6 +19885,9 @@
       <c r="D10" s="14" t="s">
         <v>83</v>
       </c>
+      <c r="G10" s="11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -19867,6 +19896,9 @@
       <c r="D11" s="11" t="s">
         <v>84</v>
       </c>
+      <c r="G11" s="11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
@@ -19881,6 +19913,9 @@
       <c r="F12" t="s">
         <v>1481</v>
       </c>
+      <c r="G12" s="11" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
@@ -19892,6 +19927,9 @@
       <c r="D13" s="12" t="s">
         <v>98</v>
       </c>
+      <c r="G13" s="11" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
@@ -19903,6 +19941,9 @@
       <c r="D14" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="G14" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
@@ -19914,6 +19955,9 @@
       <c r="D15" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="G15" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -19923,47 +19967,62 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>49</v>
       </c>
+      <c r="G17" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>55</v>
       </c>
+      <c r="G18" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>28</v>
       </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="G20" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>36</v>
       </c>
+      <c r="G21" s="12" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -19976,24 +20035,33 @@
       <c r="F22" t="s">
         <v>1475</v>
       </c>
+      <c r="G22" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>54</v>
       </c>
+      <c r="G23" s="12" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>97</v>
       </c>
+      <c r="G24" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
@@ -20003,16 +20071,22 @@
       <c r="E25" t="s">
         <v>1472</v>
       </c>
+      <c r="G25" s="12" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>16</v>
       </c>
+      <c r="G26" s="12" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -20022,16 +20096,22 @@
       <c r="E27" t="s">
         <v>1472</v>
       </c>
+      <c r="G27" s="12" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>31</v>
       </c>
+      <c r="G28" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>65</v>
       </c>
@@ -20041,16 +20121,22 @@
       <c r="D29" s="11" t="s">
         <v>77</v>
       </c>
+      <c r="G29" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>63</v>
       </c>
+      <c r="G30" s="12" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
@@ -20058,15 +20144,18 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>82</v>
       </c>
+      <c r="G32" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>75</v>
       </c>
@@ -20076,8 +20165,11 @@
       <c r="D33" s="12" t="s">
         <v>92</v>
       </c>
+      <c r="G33" s="14" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>76</v>
       </c>
@@ -20087,40 +20179,55 @@
       <c r="D34" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="G34" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>58</v>
       </c>
+      <c r="G35" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="G36" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>66</v>
       </c>
+      <c r="G37" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="G38" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>84</v>
       </c>
@@ -20130,8 +20237,11 @@
       <c r="D39" s="14" t="s">
         <v>0</v>
       </c>
+      <c r="G39" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
@@ -20139,8 +20249,11 @@
         <v>81</v>
       </c>
       <c r="E40" s="13"/>
+      <c r="G40" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -20150,24 +20263,33 @@
       <c r="E41" t="s">
         <v>1473</v>
       </c>
+      <c r="G41" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="G42" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="G43" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
@@ -20177,32 +20299,44 @@
       <c r="E44" t="s">
         <v>1472</v>
       </c>
+      <c r="G44" s="14" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="G45" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>1</v>
       </c>
+      <c r="G46" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="G47" s="14" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -20212,16 +20346,22 @@
       <c r="E48" t="s">
         <v>1472</v>
       </c>
+      <c r="G48" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="G49" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
@@ -20231,37 +20371,19 @@
       <c r="E50" t="s">
         <v>1472</v>
       </c>
-      <c r="G50">
-        <v>15</v>
-      </c>
-      <c r="H50">
-        <v>45</v>
-      </c>
-      <c r="I50">
-        <v>20</v>
-      </c>
-      <c r="J50">
-        <v>60</v>
+      <c r="G50" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D51" s="15">
         <v>44210</v>
       </c>
-      <c r="G51">
-        <v>15</v>
-      </c>
-      <c r="H51">
-        <v>45</v>
-      </c>
-      <c r="I51">
-        <v>20</v>
-      </c>
-      <c r="J51">
-        <v>60</v>
+      <c r="G51" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>31</v>
       </c>
@@ -20274,34 +20396,16 @@
       <c r="F52" t="s">
         <v>1477</v>
       </c>
-      <c r="G52">
-        <v>20</v>
-      </c>
-      <c r="H52">
-        <v>20</v>
-      </c>
-      <c r="I52">
-        <v>20</v>
-      </c>
-      <c r="J52">
-        <v>20</v>
+      <c r="G52" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D53" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G53">
-        <v>50</v>
-      </c>
-      <c r="H53">
-        <v>110</v>
-      </c>
-      <c r="J53">
-        <v>140</v>
-      </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D54" s="11" t="s">
         <v>21</v>
       </c>
@@ -20312,42 +20416,42 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D55" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D56" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D57" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D58" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D59" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D60" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D61" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D62" s="1" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Piloting the new version, with only 1 repetition for Old and Lures
</commit_message>
<xml_diff>
--- a/Analysis/Sound_data.xlsx
+++ b/Analysis/Sound_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC5A8EB4-5B91-4E0E-9232-B4C1CD66717B}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:40009_{FBA52542-4096-4A72-9C5C-74038B7573E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7DE9D999-9764-4AF8-AD83-3ADF99D92FCE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4416" uniqueCount="1482">
   <si>
     <t>Initial/NoRepeat/Droplet_B.wav</t>
   </si>
@@ -5370,9 +5370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV93"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
+    <sheetView topLeftCell="BI1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BH1" sqref="BH1:BH1048576"/>
+      <selection pane="bottomLeft" activeCell="BK1" sqref="BK1:BN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19699,10 +19699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F85263D-95D4-4235-A601-C901960AD746}">
-  <dimension ref="A1:BO62"/>
+  <dimension ref="A1:BO66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19983,7 +19983,7 @@
         <v>36</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>12</v>
@@ -19993,8 +19993,8 @@
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>28</v>
+      <c r="D19" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>14</v>
@@ -20004,8 +20004,8 @@
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>45</v>
+      <c r="D20" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>61</v>
@@ -20015,8 +20015,8 @@
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>36</v>
+      <c r="D21" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>98</v>
@@ -20026,8 +20026,8 @@
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>38</v>
+      <c r="D22" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E22" t="s">
         <v>1474</v>
@@ -20043,8 +20043,8 @@
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>54</v>
+      <c r="D23" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>97</v>
@@ -20055,7 +20055,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>52</v>
@@ -20065,8 +20065,8 @@
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>52</v>
+      <c r="D25" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E25" t="s">
         <v>1472</v>
@@ -20079,8 +20079,8 @@
       <c r="A26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>16</v>
+      <c r="D26" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>82</v>
@@ -20090,8 +20090,8 @@
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>46</v>
+      <c r="D27" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="E27" t="s">
         <v>1472</v>
@@ -20104,8 +20104,8 @@
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>31</v>
+      <c r="D28" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>8</v>
@@ -20118,8 +20118,8 @@
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>77</v>
+      <c r="D29" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>6</v>
@@ -20130,7 +20130,7 @@
         <v>66</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>94</v>
@@ -20140,8 +20140,8 @@
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>69</v>
+      <c r="D31" s="12" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -20149,7 +20149,7 @@
         <v>73</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>27</v>
@@ -20163,7 +20163,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>83</v>
@@ -20176,8 +20176,8 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>8</v>
+      <c r="D34" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>17</v>
@@ -20187,8 +20187,8 @@
       <c r="A35" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>58</v>
+      <c r="D35" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="G35" s="14" t="s">
         <v>48</v>
@@ -20198,8 +20198,8 @@
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>78</v>
+      <c r="D36" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>49</v>
@@ -20209,8 +20209,8 @@
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>66</v>
+      <c r="D37" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>55</v>
@@ -20220,8 +20220,8 @@
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>71</v>
+      <c r="D38" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="G38" s="14" t="s">
         <v>28</v>
@@ -20234,8 +20234,8 @@
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>0</v>
+      <c r="D39" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>36</v>
@@ -20245,8 +20245,8 @@
       <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>81</v>
+      <c r="D40" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="E40" s="13"/>
       <c r="G40" s="14" t="s">
@@ -20257,8 +20257,8 @@
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>10</v>
+      <c r="D41" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E41" t="s">
         <v>1473</v>
@@ -20271,8 +20271,8 @@
       <c r="A42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>35</v>
+      <c r="D42" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>31</v>
@@ -20282,8 +20282,8 @@
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>5</v>
+      <c r="D43" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>63</v>
@@ -20294,7 +20294,7 @@
         <v>94</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
         <v>1472</v>
@@ -20307,8 +20307,8 @@
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>89</v>
+      <c r="D45" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>78</v>
@@ -20318,8 +20318,8 @@
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>1</v>
+      <c r="D46" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>71</v>
@@ -20329,8 +20329,8 @@
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>57</v>
+      <c r="D47" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="G47" s="14" t="s">
         <v>0</v>
@@ -20341,7 +20341,7 @@
         <v>10</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="E48" t="s">
         <v>1472</v>
@@ -20354,8 +20354,14 @@
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>62</v>
+      <c r="D49" s="15">
+        <v>44210</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1478</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>35</v>
@@ -20365,8 +20371,8 @@
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>94</v>
+      <c r="D50" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="E50" t="s">
         <v>1472</v>
@@ -20376,8 +20382,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D51" s="15">
-        <v>44210</v>
+      <c r="D51" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>89</v>
@@ -20387,8 +20393,8 @@
       <c r="A52" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>67</v>
+      <c r="D52" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E52" t="s">
         <v>1476</v>
@@ -20401,59 +20407,73 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D53" s="7" t="s">
-        <v>22</v>
+      <c r="D53" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D54" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E54" t="s">
-        <v>1479</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1478</v>
+      <c r="D54" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D55" s="1" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D56" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D57" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D58" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D59" s="1" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D60" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D61" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D62" s="1" t="s">
-        <v>96</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D64" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D65" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D66" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>